<commit_message>
Removed 2 redundant arguments from meta-measure.
By storing the measure dir in _options_lookup.txt, different measures
can be referenced within a single input distribution (e.g., air
conditioner vs heat pump for cooling systems).
</commit_message>
<xml_diff>
--- a/projects/national scale/res_stock.xlsx
+++ b/projects/national scale/res_stock.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="312">
   <si>
     <t>type</t>
   </si>
@@ -929,33 +929,15 @@
     <t>CallMetaMeasure</t>
   </si>
   <si>
-    <t>dependencies</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
-    <t>Set Dependencies</t>
-  </si>
-  <si>
     <t>Set Sample Value</t>
   </si>
   <si>
     <t>sample_value</t>
   </si>
   <si>
-    <t>Set Measure Dir</t>
-  </si>
-  <si>
-    <t>measure_dir</t>
-  </si>
-  <si>
-    <t>SetResidentialEPWFile</t>
-  </si>
-  <si>
-    <t>ProcessConstructionsWallsExteriorWoodStud</t>
-  </si>
-  <si>
     <t>Set Parameter Name</t>
   </si>
   <si>
@@ -969,9 +951,6 @@
   </si>
   <si>
     <t>ExteriorWalls</t>
-  </si>
-  <si>
-    <t>Location|Vintage</t>
   </si>
   <si>
     <t>Set Probability Distributions File</t>
@@ -5209,10 +5188,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z70"/>
+  <dimension ref="A1:Z64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5395,7 +5374,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>295</v>
@@ -5414,18 +5393,18 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -5445,25 +5424,25 @@
       <c r="Y5" s="15"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -5483,222 +5462,199 @@
       <c r="Y6" s="15"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="I7" s="39">
+        <v>50</v>
+      </c>
+      <c r="K7" s="39">
+        <v>1</v>
+      </c>
+      <c r="L7" s="39">
+        <v>100</v>
+      </c>
+      <c r="M7" s="39">
+        <v>50</v>
+      </c>
+      <c r="N7" s="39">
+        <v>16.66667</v>
+      </c>
+      <c r="R7" s="39" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>310</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>295</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>295</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+    </row>
+    <row r="10" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+    </row>
+    <row r="11" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="I11" s="39">
+        <v>50</v>
+      </c>
+      <c r="K11" s="39">
+        <v>1</v>
+      </c>
+      <c r="L11" s="39">
+        <v>100</v>
+      </c>
+      <c r="M11" s="39">
+        <v>50</v>
+      </c>
+      <c r="N11" s="39">
+        <v>16.66667</v>
+      </c>
+      <c r="R11" s="39" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="37" t="s">
         <v>311</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
-    </row>
-    <row r="8" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-    </row>
-    <row r="9" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>299</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>300</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="I9" s="39">
-        <v>50</v>
-      </c>
-      <c r="K9" s="39">
-        <v>1</v>
-      </c>
-      <c r="L9" s="39">
-        <v>100</v>
-      </c>
-      <c r="M9" s="39">
-        <v>50</v>
-      </c>
-      <c r="N9" s="39">
-        <v>16.66667</v>
-      </c>
-      <c r="R9" s="39" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>317</v>
-      </c>
-      <c r="C10" s="37" t="s">
+      <c r="C12" s="37" t="s">
         <v>295</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D12" s="37" t="s">
         <v>295</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E12" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-    </row>
-    <row r="12" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-    </row>
-    <row r="13" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -5718,25 +5674,25 @@
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -5761,10 +5717,10 @@
         <v>21</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G15" s="39" t="s">
         <v>175</v>
@@ -5788,43 +5744,44 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>318</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>295</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>295</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+    </row>
+    <row r="17" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
-      <c r="B17" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="B17" s="10"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>306</v>
-      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="10" t="s">
-        <v>297</v>
-      </c>
+      <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="10" t="s">
-        <v>309</v>
-      </c>
+      <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
@@ -5843,26 +5800,16 @@
       <c r="Y17" s="15"/>
       <c r="Z17" s="15"/>
     </row>
-    <row r="18" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
-      <c r="B18" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="B18" s="10"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>302</v>
-      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="10" t="s">
-        <v>297</v>
-      </c>
+      <c r="G18" s="10"/>
       <c r="H18" s="10"/>
-      <c r="I18" s="10" t="s">
-        <v>304</v>
-      </c>
+      <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
@@ -5881,26 +5828,16 @@
       <c r="Y18" s="15"/>
       <c r="Z18" s="15"/>
     </row>
-    <row r="19" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="B19" s="10"/>
       <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>312</v>
-      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
-        <v>297</v>
-      </c>
+      <c r="G19" s="10"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="10" t="s">
-        <v>315</v>
-      </c>
+      <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -5919,26 +5856,16 @@
       <c r="Y19" s="15"/>
       <c r="Z19" s="15"/>
     </row>
-    <row r="20" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="B20" s="10"/>
       <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>296</v>
-      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="10" t="s">
-        <v>297</v>
-      </c>
+      <c r="G20" s="10"/>
       <c r="H20" s="10"/>
-      <c r="I20" s="10" t="s">
-        <v>310</v>
-      </c>
+      <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
@@ -5957,39 +5884,35 @@
       <c r="Y20" s="15"/>
       <c r="Z20" s="15"/>
     </row>
-    <row r="21" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>299</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>300</v>
-      </c>
-      <c r="G21" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="I21" s="39">
-        <v>50</v>
-      </c>
-      <c r="K21" s="39">
-        <v>1</v>
-      </c>
-      <c r="L21" s="39">
-        <v>100</v>
-      </c>
-      <c r="M21" s="39">
-        <v>50</v>
-      </c>
-      <c r="N21" s="39">
-        <v>16.66667</v>
-      </c>
-      <c r="R21" s="39" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -6030,11 +5953,11 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="38"/>
       <c r="R23" s="15"/>
       <c r="S23" s="15"/>
       <c r="T23" s="15"/>
@@ -6045,8 +5968,8 @@
       <c r="Y23" s="15"/>
       <c r="Z23" s="15"/>
     </row>
-    <row r="24" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+    <row r="24" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -6073,7 +5996,7 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -6086,7 +6009,7 @@
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
-      <c r="M25" s="15"/>
+      <c r="M25" s="10"/>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
@@ -6101,7 +6024,7 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
     </row>
-    <row r="26" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -6114,11 +6037,11 @@
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
       <c r="R26" s="15"/>
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
@@ -6129,7 +6052,7 @@
       <c r="Y26" s="15"/>
       <c r="Z26" s="15"/>
     </row>
-    <row r="27" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -6170,7 +6093,7 @@
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
-      <c r="M28" s="15"/>
+      <c r="M28" s="10"/>
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
@@ -6185,7 +6108,7 @@
       <c r="Y28" s="15"/>
       <c r="Z28" s="15"/>
     </row>
-    <row r="29" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -6381,19 +6304,19 @@
       <c r="Y35" s="15"/>
       <c r="Z35" s="15"/>
     </row>
-    <row r="36" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
@@ -6409,20 +6332,20 @@
       <c r="Y36" s="15"/>
       <c r="Z36" s="15"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
       <c r="P37" s="15"/>
@@ -6437,24 +6360,24 @@
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="38"/>
-      <c r="N38" s="38"/>
-      <c r="O38" s="38"/>
-      <c r="P38" s="38"/>
-      <c r="Q38" s="38"/>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
       <c r="S38" s="15"/>
       <c r="T38" s="15"/>
@@ -6465,23 +6388,23 @@
       <c r="Y38" s="15"/>
       <c r="Z38" s="15"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
+      <c r="O39" s="38"/>
+      <c r="P39" s="38"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
       <c r="S39" s="15"/>
@@ -6493,20 +6416,20 @@
       <c r="Y39" s="15"/>
       <c r="Z39" s="15"/>
     </row>
-    <row r="40" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
       <c r="P40" s="15"/>
@@ -6521,24 +6444,24 @@
       <c r="Y40" s="15"/>
       <c r="Z40" s="15"/>
     </row>
-    <row r="41" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="38"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="38"/>
-      <c r="Q41" s="38"/>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
       <c r="S41" s="15"/>
       <c r="T41" s="15"/>
@@ -6633,7 +6556,7 @@
       <c r="Y44" s="15"/>
       <c r="Z44" s="15"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -6647,7 +6570,7 @@
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
+      <c r="N45" s="10"/>
       <c r="O45" s="38"/>
       <c r="P45" s="38"/>
       <c r="Q45" s="15"/>
@@ -6801,7 +6724,7 @@
       <c r="Y50" s="15"/>
       <c r="Z50" s="15"/>
     </row>
-    <row r="51" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
@@ -6815,9 +6738,9 @@
       <c r="K51" s="15"/>
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
-      <c r="N51" s="10"/>
-      <c r="O51" s="38"/>
-      <c r="P51" s="38"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
       <c r="Q51" s="15"/>
       <c r="R51" s="15"/>
       <c r="S51" s="15"/>
@@ -6829,8 +6752,8 @@
       <c r="Y51" s="15"/>
       <c r="Z51" s="15"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+    <row r="52" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
@@ -6844,8 +6767,8 @@
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
-      <c r="O52" s="15"/>
-      <c r="P52" s="15"/>
+      <c r="O52" s="38"/>
+      <c r="P52" s="38"/>
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
       <c r="S52" s="15"/>
@@ -6900,8 +6823,8 @@
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
       <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
+      <c r="O54" s="38"/>
+      <c r="P54" s="38"/>
       <c r="Q54" s="15"/>
       <c r="R54" s="15"/>
       <c r="S54" s="15"/>
@@ -6928,8 +6851,8 @@
       <c r="L55" s="15"/>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
+      <c r="O55" s="38"/>
+      <c r="P55" s="38"/>
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
       <c r="S55" s="15"/>
@@ -6984,8 +6907,8 @@
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
-      <c r="P57" s="15"/>
+      <c r="O57" s="38"/>
+      <c r="P57" s="38"/>
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
       <c r="S57" s="15"/>
@@ -6997,8 +6920,8 @@
       <c r="Y57" s="15"/>
       <c r="Z57" s="15"/>
     </row>
-    <row r="58" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A58" s="15"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
@@ -7012,8 +6935,8 @@
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
-      <c r="O58" s="38"/>
-      <c r="P58" s="38"/>
+      <c r="O58" s="15"/>
+      <c r="P58" s="15"/>
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
       <c r="S58" s="15"/>
@@ -7040,8 +6963,8 @@
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
-      <c r="O59" s="15"/>
-      <c r="P59" s="15"/>
+      <c r="O59" s="38"/>
+      <c r="P59" s="38"/>
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
       <c r="S59" s="15"/>
@@ -7068,8 +6991,8 @@
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
       <c r="N60" s="15"/>
-      <c r="O60" s="38"/>
-      <c r="P60" s="38"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="15"/>
       <c r="Q60" s="15"/>
       <c r="R60" s="15"/>
       <c r="S60" s="15"/>
@@ -7192,174 +7115,6 @@
       <c r="X64" s="15"/>
       <c r="Y64" s="15"/>
       <c r="Z64" s="15"/>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="15"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="38"/>
-      <c r="P65" s="38"/>
-      <c r="Q65" s="15"/>
-      <c r="R65" s="15"/>
-      <c r="S65" s="15"/>
-      <c r="T65" s="15"/>
-      <c r="U65" s="15"/>
-      <c r="V65" s="15"/>
-      <c r="W65" s="15"/>
-      <c r="X65" s="15"/>
-      <c r="Y65" s="15"/>
-      <c r="Z65" s="15"/>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="15"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="15"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="15"/>
-      <c r="O66" s="15"/>
-      <c r="P66" s="15"/>
-      <c r="Q66" s="15"/>
-      <c r="R66" s="15"/>
-      <c r="S66" s="15"/>
-      <c r="T66" s="15"/>
-      <c r="U66" s="15"/>
-      <c r="V66" s="15"/>
-      <c r="W66" s="15"/>
-      <c r="X66" s="15"/>
-      <c r="Y66" s="15"/>
-      <c r="Z66" s="15"/>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
-      <c r="B67" s="15"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="15"/>
-      <c r="L67" s="15"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="15"/>
-      <c r="O67" s="38"/>
-      <c r="P67" s="38"/>
-      <c r="Q67" s="15"/>
-      <c r="R67" s="15"/>
-      <c r="S67" s="15"/>
-      <c r="T67" s="15"/>
-      <c r="U67" s="15"/>
-      <c r="V67" s="15"/>
-      <c r="W67" s="15"/>
-      <c r="X67" s="15"/>
-      <c r="Y67" s="15"/>
-      <c r="Z67" s="15"/>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="15"/>
-      <c r="I68" s="15"/>
-      <c r="J68" s="15"/>
-      <c r="K68" s="15"/>
-      <c r="L68" s="15"/>
-      <c r="M68" s="15"/>
-      <c r="N68" s="15"/>
-      <c r="O68" s="15"/>
-      <c r="P68" s="15"/>
-      <c r="Q68" s="15"/>
-      <c r="R68" s="15"/>
-      <c r="S68" s="15"/>
-      <c r="T68" s="15"/>
-      <c r="U68" s="15"/>
-      <c r="V68" s="15"/>
-      <c r="W68" s="15"/>
-      <c r="X68" s="15"/>
-      <c r="Y68" s="15"/>
-      <c r="Z68" s="15"/>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-      <c r="J69" s="15"/>
-      <c r="K69" s="15"/>
-      <c r="L69" s="15"/>
-      <c r="M69" s="15"/>
-      <c r="N69" s="15"/>
-      <c r="O69" s="38"/>
-      <c r="P69" s="38"/>
-      <c r="Q69" s="15"/>
-      <c r="R69" s="15"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="15"/>
-      <c r="U69" s="15"/>
-      <c r="V69" s="15"/>
-      <c r="W69" s="15"/>
-      <c r="X69" s="15"/>
-      <c r="Y69" s="15"/>
-      <c r="Z69" s="15"/>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="15"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="15"/>
-      <c r="K70" s="15"/>
-      <c r="L70" s="15"/>
-      <c r="M70" s="15"/>
-      <c r="N70" s="15"/>
-      <c r="O70" s="15"/>
-      <c r="P70" s="15"/>
-      <c r="Q70" s="15"/>
-      <c r="R70" s="15"/>
-      <c r="S70" s="15"/>
-      <c r="T70" s="15"/>
-      <c r="U70" s="15"/>
-      <c r="V70" s="15"/>
-      <c r="W70" s="15"/>
-      <c r="X70" s="15"/>
-      <c r="Y70" s="15"/>
-      <c r="Z70" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>

</xml_diff>